<commit_message>
* Updated GDD to 1.3.1
* Updated  TTCh-table  example
</commit_message>
<xml_diff>
--- a/UnityProject-4/Пример таблицы ТТХ.xlsx
+++ b/UnityProject-4/Пример таблицы ТТХ.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Лист3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
   <si>
     <t>ConArmHEAT</t>
   </si>
@@ -146,9 +145,6 @@
     <t>RefArmPHYS</t>
   </si>
   <si>
-    <t xml:space="preserve">       Cost</t>
-  </si>
-  <si>
     <t xml:space="preserve">          Damage</t>
   </si>
   <si>
@@ -158,9 +154,6 @@
     <t>unit_workname</t>
   </si>
   <si>
-    <t xml:space="preserve"> Motion</t>
-  </si>
-  <si>
     <t>missile_launcher</t>
   </si>
   <si>
@@ -267,6 +260,33 @@
   </si>
   <si>
     <t>Allows usage of Homing Valley. \n Charges for {BoostChargingTime} seconds after which first fired valley will have homing ability.</t>
+  </si>
+  <si>
+    <t>sight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Economy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Boost</t>
+  </si>
+  <si>
+    <t>stack_stun</t>
+  </si>
+  <si>
+    <t>stack_overheat</t>
+  </si>
+  <si>
+    <t>stack_destabilization</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Aiming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Motion</t>
   </si>
 </sst>
 </file>
@@ -303,10 +323,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L61"/>
+  <dimension ref="B1:L67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,92 +1351,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" t="s">
         <v>62</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J3" t="s">
         <v>63</v>
       </c>
-      <c r="L1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>64</v>
       </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" t="s">
-        <v>66</v>
-      </c>
       <c r="L3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
@@ -1433,9 +1459,6 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
@@ -1449,17 +1472,11 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>0.5</v>
-      </c>
-    </row>
+    <row r="8" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
@@ -1495,9 +1512,7 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="B13" s="1"/>
       <c r="C13" t="s">
         <v>2</v>
       </c>
@@ -1514,402 +1529,477 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" t="s">
+    <row r="15" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="L16">
         <v>6</v>
       </c>
-      <c r="E15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
       <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="L17">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
       <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="L18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" t="s">
         <v>33</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>36</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
       <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>26</v>
       </c>
-      <c r="E26">
+      <c r="E29">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>27</v>
       </c>
-      <c r="E27">
+      <c r="E30">
         <v>0.7</v>
       </c>
-      <c r="J27">
+      <c r="J30">
         <v>0.1</v>
       </c>
-      <c r="K27">
+      <c r="K30">
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>28</v>
       </c>
-      <c r="E28">
+      <c r="E31">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>31</v>
       </c>
-      <c r="E29">
+      <c r="E32">
         <v>4</v>
       </c>
-      <c r="G29">
+      <c r="G32">
         <v>1</v>
       </c>
-      <c r="H29">
+      <c r="H32">
         <v>1</v>
       </c>
-      <c r="I29">
+      <c r="I32">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>29</v>
       </c>
-      <c r="E30">
+      <c r="E33">
         <v>2</v>
       </c>
-      <c r="G30">
+      <c r="G33">
         <v>1</v>
       </c>
-      <c r="H30">
+      <c r="H33">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>30</v>
       </c>
-      <c r="E31">
+      <c r="E34">
         <v>0.4</v>
       </c>
-      <c r="G31">
+      <c r="G34">
         <v>0.4</v>
       </c>
-      <c r="H31">
+      <c r="H34">
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>25</v>
       </c>
-      <c r="E32">
+      <c r="E35">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>76</v>
-      </c>
-      <c r="L34">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>77</v>
-      </c>
-      <c r="L35">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>78</v>
-      </c>
-      <c r="L36">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>44</v>
-      </c>
+    <row r="37" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
       <c r="C38" t="s">
         <v>19</v>
       </c>
       <c r="E38">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
       <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
         <v>14</v>
       </c>
-      <c r="E41">
+      <c r="E43">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>12</v>
       </c>
-      <c r="E42" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C44" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-      <c r="C45" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
+      <c r="E44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="C46" t="s">
         <v>47</v>
       </c>
       <c r="E46">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E47">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="C48" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E48">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="C49" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E49">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E50">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E51">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E52">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+      <c r="C53" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+      <c r="C54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" t="s">
         <v>24</v>
       </c>
-      <c r="E54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+      <c r="E56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+      <c r="C57" t="s">
         <v>21</v>
       </c>
-      <c r="E55">
+      <c r="E57">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+    <row r="58" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="1"/>
+      <c r="C58" t="s">
         <v>20</v>
       </c>
-      <c r="E56">
+      <c r="E58">
         <v>30</v>
       </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+      <c r="J58" s="2"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="1"/>
+      <c r="C59" t="s">
         <v>22</v>
       </c>
-      <c r="E57">
+      <c r="E59">
         <v>-45</v>
       </c>
-      <c r="F57">
+      <c r="F59">
         <v>45</v>
       </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+      <c r="C60" t="s">
         <v>23</v>
       </c>
-      <c r="E58">
+      <c r="E60">
         <v>0</v>
       </c>
-      <c r="F58">
+      <c r="F60">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+      <c r="J60" s="2"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J61" s="2"/>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="1"/>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="1"/>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="1"/>
+      <c r="C65" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="1"/>
+      <c r="C66" t="s">
         <v>17</v>
       </c>
-      <c r="E60">
+      <c r="E66">
         <v>0.4</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+      <c r="C67" t="s">
         <v>18</v>
       </c>
-      <c r="E61">
+      <c r="E67">
         <v>0.4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="B44:B52"/>
+  <mergeCells count="7">
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="B46:B54"/>
+    <mergeCell ref="B62:B67"/>
+    <mergeCell ref="B16:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
* Updated GDD to 1.4 and Units TTCh
</commit_message>
<xml_diff>
--- a/UnityProject-4/Пример таблицы ТТХ.xlsx
+++ b/UnityProject-4/Пример таблицы ТТХ.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="94">
   <si>
     <t>ConArmHEAT</t>
   </si>
@@ -37,108 +37,9 @@
     <t>RefArmEN</t>
   </si>
   <si>
-    <t>cost_SM</t>
-  </si>
-  <si>
-    <t>cost_energy</t>
-  </si>
-  <si>
-    <t>cost_parts</t>
-  </si>
-  <si>
     <t>speed</t>
   </si>
   <si>
-    <t>reverse_factor</t>
-  </si>
-  <si>
-    <t>hp_max</t>
-  </si>
-  <si>
-    <t>hp_wreckage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">             Armor</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
-    <t>basic_build_time</t>
-  </si>
-  <si>
-    <t>deploy_radius</t>
-  </si>
-  <si>
-    <t>rotation_speed</t>
-  </si>
-  <si>
-    <t>acceleration</t>
-  </si>
-  <si>
-    <t>recovery_parts_factor</t>
-  </si>
-  <si>
-    <t>recovery_energy_factor</t>
-  </si>
-  <si>
-    <t>optimal distance</t>
-  </si>
-  <si>
-    <t>vert_rotation_speed</t>
-  </si>
-  <si>
-    <t>hor_rotation_speed</t>
-  </si>
-  <si>
-    <t>hor_shooting_zone</t>
-  </si>
-  <si>
-    <t>vert_shooting_zone</t>
-  </si>
-  <si>
-    <t>aim_type</t>
-  </si>
-  <si>
-    <t>muzzle_velocity</t>
-  </si>
-  <si>
-    <t>range</t>
-  </si>
-  <si>
-    <t>accuracy</t>
-  </si>
-  <si>
-    <t>aoe</t>
-  </si>
-  <si>
-    <t>shots</t>
-  </si>
-  <si>
-    <t>shots_time</t>
-  </si>
-  <si>
-    <t>reload_time</t>
-  </si>
-  <si>
-    <t>dmg_PHYS</t>
-  </si>
-  <si>
-    <t>dmg_HEAT</t>
-  </si>
-  <si>
-    <t>dmg_EN</t>
-  </si>
-  <si>
-    <t>piercing_PHYS</t>
-  </si>
-  <si>
-    <t>piercing_HEAT</t>
-  </si>
-  <si>
-    <t>piercing_EN</t>
-  </si>
-  <si>
     <t>ConArmPHYS</t>
   </si>
   <si>
@@ -148,42 +49,6 @@
     <t xml:space="preserve">          Damage</t>
   </si>
   <si>
-    <t>unit_name</t>
-  </si>
-  <si>
-    <t>unit_workname</t>
-  </si>
-  <si>
-    <t>missile_launcher</t>
-  </si>
-  <si>
-    <t>unit_description</t>
-  </si>
-  <si>
-    <t>heavy_materiel</t>
-  </si>
-  <si>
-    <t>light_materiel</t>
-  </si>
-  <si>
-    <t>infantry</t>
-  </si>
-  <si>
-    <t>artillery</t>
-  </si>
-  <si>
-    <t>light_air</t>
-  </si>
-  <si>
-    <t>heavy_air</t>
-  </si>
-  <si>
-    <t>building</t>
-  </si>
-  <si>
-    <t>SC</t>
-  </si>
-  <si>
     <t xml:space="preserve">                    Priorities</t>
   </si>
   <si>
@@ -193,24 +58,6 @@
     <t>"Viper" is a true missile launcher - fragile, but carrying good payload and quite mobile.</t>
   </si>
   <si>
-    <t>trajectory_missile</t>
-  </si>
-  <si>
-    <t>UpgSHOTS-1</t>
-  </si>
-  <si>
-    <t>UpgSHOTS-2</t>
-  </si>
-  <si>
-    <t>UpgRELOAD-1</t>
-  </si>
-  <si>
-    <t>UpgACC-1</t>
-  </si>
-  <si>
-    <t>UpgACC-2</t>
-  </si>
-  <si>
     <t>Additional hydraulics increases "Viper's" rate of fire.</t>
   </si>
   <si>
@@ -238,15 +85,9 @@
     <t>Viper is equipped with additional rail allowing it to lauch more missiles at once. This slightly increases reload time, however</t>
   </si>
   <si>
-    <t>UpgHOMING-1</t>
-  </si>
-  <si>
     <t>Homing valley</t>
   </si>
   <si>
-    <t>upgrade_requirements</t>
-  </si>
-  <si>
     <t>BoostChargingTime</t>
   </si>
   <si>
@@ -262,31 +103,208 @@
     <t>Allows usage of Homing Valley. \n Charges for {BoostChargingTime} seconds after which first fired valley will have homing ability.</t>
   </si>
   <si>
-    <t>sight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          Economy</t>
-  </si>
-  <si>
     <t xml:space="preserve">            Boost</t>
   </si>
   <si>
-    <t>stack_stun</t>
-  </si>
-  <si>
-    <t>stack_overheat</t>
-  </si>
-  <si>
-    <t>stack_destabilization</t>
-  </si>
-  <si>
-    <t>mass</t>
-  </si>
-  <si>
     <t xml:space="preserve">        Aiming</t>
   </si>
   <si>
     <t xml:space="preserve">           Motion</t>
+  </si>
+  <si>
+    <t>[10,parts]_[1,energy]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Economy</t>
+  </si>
+  <si>
+    <t>HpRegen</t>
+  </si>
+  <si>
+    <t>HpWreckage</t>
+  </si>
+  <si>
+    <t>HpMax</t>
+  </si>
+  <si>
+    <t>UpgradeRequirements</t>
+  </si>
+  <si>
+    <t>UnitWorkname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               Armor</t>
+  </si>
+  <si>
+    <t>AoeFactor</t>
+  </si>
+  <si>
+    <t>StackStun</t>
+  </si>
+  <si>
+    <t>StackOverheat</t>
+  </si>
+  <si>
+    <t>StackDestabilization</t>
+  </si>
+  <si>
+    <t>DmgPHYS</t>
+  </si>
+  <si>
+    <t>DmgHEAT</t>
+  </si>
+  <si>
+    <t>DmgEN</t>
+  </si>
+  <si>
+    <t>PiercingPHYS</t>
+  </si>
+  <si>
+    <t>PiercingHEAT</t>
+  </si>
+  <si>
+    <t>PiercingEN</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>AoeRadius</t>
+  </si>
+  <si>
+    <t>ReloadTime</t>
+  </si>
+  <si>
+    <t>ShotsTime</t>
+  </si>
+  <si>
+    <t>MuzzleVelocity</t>
+  </si>
+  <si>
+    <t>Sight</t>
+  </si>
+  <si>
+    <t>OptimalDistance</t>
+  </si>
+  <si>
+    <t>Acceleration</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>ReverseFactor</t>
+  </si>
+  <si>
+    <t>DeployRadius</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Infantry</t>
+  </si>
+  <si>
+    <t>LightMateriel</t>
+  </si>
+  <si>
+    <t>HeavyMateriel</t>
+  </si>
+  <si>
+    <t>MissileLauncher</t>
+  </si>
+  <si>
+    <t>Artillery</t>
+  </si>
+  <si>
+    <t>LightAir</t>
+  </si>
+  <si>
+    <t>HeavyAir</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>CostParts</t>
+  </si>
+  <si>
+    <t>CostEnergy</t>
+  </si>
+  <si>
+    <t>CostSM</t>
+  </si>
+  <si>
+    <t>BasicBuildTime</t>
+  </si>
+  <si>
+    <t>Recovery</t>
+  </si>
+  <si>
+    <t>AimType</t>
+  </si>
+  <si>
+    <t>HorRotationSpeed</t>
+  </si>
+  <si>
+    <t>VertRotationSpeed</t>
+  </si>
+  <si>
+    <t>HorShootingZone</t>
+  </si>
+  <si>
+    <t>VertShootingZone</t>
+  </si>
+  <si>
+    <t>UnitName</t>
+  </si>
+  <si>
+    <t>UnitDescription</t>
+  </si>
+  <si>
+    <t>UpgShots2</t>
+  </si>
+  <si>
+    <t>UpgShots1</t>
+  </si>
+  <si>
+    <t>UpgReload1</t>
+  </si>
+  <si>
+    <t>UpgAcc1</t>
+  </si>
+  <si>
+    <t>UpgAcc2</t>
+  </si>
+  <si>
+    <t>UpgHoming1</t>
+  </si>
+  <si>
+    <t>[7,BoostHoming]</t>
+  </si>
+  <si>
+    <t>[3,BoostHoming]</t>
+  </si>
+  <si>
+    <t>ShotsAmount</t>
+  </si>
+  <si>
+    <t>TrajectoryMissile</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>1-60 - left track motion;   121-180 - right track motion;    241-300 - shooting</t>
+  </si>
+  <si>
+    <t>TurnSpeed</t>
   </si>
 </sst>
 </file>
@@ -326,10 +344,10 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+      <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="90"/>
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1330,320 +1348,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L67"/>
+  <dimension ref="B1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="2"/>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="J1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="K1" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="L1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
+        <v>86</v>
+      </c>
+      <c r="M1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3">
         <v>70</v>
       </c>
-      <c r="H3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7">
         <v>3</v>
       </c>
-      <c r="G7">
+      <c r="G6">
         <v>-0.25</v>
       </c>
-      <c r="H7">
+      <c r="H6">
         <v>-0.25</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
+    <row r="8" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="E14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="L16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="L17">
         <v>17.5</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="L18">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
       <c r="C19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
         <v>40</v>
       </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="E23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
+      <c r="L23" t="s">
+        <v>88</v>
+      </c>
+      <c r="M23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="E29">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="E30">
         <v>0.7</v>
@@ -1655,17 +1644,17 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -1682,7 +1671,7 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -1696,7 +1685,7 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="E34">
         <v>0.4</v>
@@ -1710,63 +1699,63 @@
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="E35">
         <v>12</v>
       </c>
     </row>
     <row r="37" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>87</v>
+      <c r="B37" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="E37">
         <v>40</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
+      <c r="B38" s="2"/>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="E38">
         <v>25</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
+      <c r="B39" s="2"/>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="E39">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
+      <c r="B40" s="2"/>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="E40">
         <v>2</v>
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
+      <c r="B41" s="2"/>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="E41">
         <v>210</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
+      <c r="B42" s="2"/>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="E42">
         <v>0.5</v>
@@ -1774,7 +1763,7 @@
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1782,224 +1771,272 @@
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="E44" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K45" s="2"/>
+      <c r="K45" s="1"/>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>53</v>
+      <c r="B46" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="E46">
         <v>2</v>
       </c>
-      <c r="K46" s="2"/>
+      <c r="K46" s="1"/>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
+      <c r="B47" s="2"/>
       <c r="C47" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E47">
         <v>10</v>
       </c>
-      <c r="K47" s="2"/>
+      <c r="K47" s="1"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
+      <c r="B48" s="2"/>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E48">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
       <c r="C49" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="E49">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="2"/>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="E50">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
       <c r="C51" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="E51">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="2"/>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="E52">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="2"/>
       <c r="C53" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E53">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="2"/>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="E54">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>86</v>
+    <row r="56" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C56" t="s">
+        <v>69</v>
+      </c>
+      <c r="E56">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="2"/>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="2"/>
+      <c r="C58" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="2"/>
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="E59">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="2"/>
+      <c r="C60" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
+      <c r="E63" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="2"/>
+      <c r="C64" t="s">
+        <v>75</v>
+      </c>
+      <c r="E64">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="2"/>
+      <c r="C65" t="s">
+        <v>76</v>
+      </c>
+      <c r="E65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="2"/>
+      <c r="C66" t="s">
+        <v>77</v>
+      </c>
+      <c r="E66">
+        <v>-45</v>
+      </c>
+      <c r="F66">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B67" s="2"/>
+      <c r="C67" t="s">
+        <v>78</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>79</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" t="s">
+        <v>18</v>
+      </c>
+      <c r="I69" t="s">
+        <v>15</v>
+      </c>
+      <c r="J69" t="s">
+        <v>16</v>
+      </c>
+      <c r="K69" t="s">
+        <v>17</v>
+      </c>
+      <c r="L69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" t="s">
+        <v>10</v>
+      </c>
+      <c r="G70" t="s">
+        <v>19</v>
+      </c>
+      <c r="H70" t="s">
         <v>24</v>
       </c>
-      <c r="E56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-      <c r="C57" t="s">
-        <v>21</v>
-      </c>
-      <c r="E57">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="C58" t="s">
-        <v>20</v>
-      </c>
-      <c r="E58">
-        <v>30</v>
-      </c>
-      <c r="J58" s="2"/>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-      <c r="C59" t="s">
-        <v>22</v>
-      </c>
-      <c r="E59">
-        <v>-45</v>
-      </c>
-      <c r="F59">
-        <v>45</v>
-      </c>
-      <c r="J59" s="2"/>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
-      <c r="C60" t="s">
-        <v>23</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60">
-        <v>60</v>
-      </c>
-      <c r="J60" s="2"/>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J61" s="2"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C62" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62">
+      <c r="I70" t="s">
+        <v>11</v>
+      </c>
+      <c r="J70" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-      <c r="C63" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B64" s="1"/>
-      <c r="C64" t="s">
-        <v>4</v>
-      </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="1"/>
-      <c r="C65" t="s">
+      <c r="K70" t="s">
         <v>13</v>
       </c>
-      <c r="E65">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="1"/>
-      <c r="C66" t="s">
-        <v>17</v>
-      </c>
-      <c r="E66">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
-      <c r="C67" t="s">
-        <v>18</v>
-      </c>
-      <c r="E67">
-        <v>0.4</v>
+      <c r="L70" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>91</v>
+      </c>
+      <c r="E72" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B16:B21"/>
     <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B8:B14"/>
+    <mergeCell ref="B63:B67"/>
     <mergeCell ref="B37:B42"/>
-    <mergeCell ref="B9:B14"/>
     <mergeCell ref="B23:B28"/>
     <mergeCell ref="B46:B54"/>
-    <mergeCell ref="B62:B67"/>
-    <mergeCell ref="B16:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
+Unit + UpgradeController + Simple UI
</commit_message>
<xml_diff>
--- a/UnityProject-4/Пример таблицы ТТХ.xlsx
+++ b/UnityProject-4/Пример таблицы ТТХ.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Project-4\UnityProject-4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="330" windowWidth="19740" windowHeight="7620"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="Лист2" sheetId="2" r:id="rId1"/>
     <sheet name="Лист3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -19,6 +24,9 @@
   <connection id="1" name="Settings" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="D:\Data(2)\Data\Settings.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
+  <connection id="2" name="Units" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="C:\Git\Project-4\UnityProject-4\Assets\Resources\Units.xml" htmlTables="1"/>
+  </connection>
 </connections>
 </file>
 
@@ -310,7 +318,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -351,13 +359,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1055,16 +1066,112 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
+  <Schema ID="Schema2">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="units">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0" maxOccurs="unbounded">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Unit" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="UnitName" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ModelName" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="IconName" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="UnitDescription" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="HpMax" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="HpWreckage" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="HpRegen" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="CostParts" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="CostEnergy" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="CostSM" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="BasicBuildTime" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="DeployRadius" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="SpeedGlobal" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Speed" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ReverseFactor" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="TurnSpeed" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Acceleration" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Mass" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Recovery" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Class" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Priority" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Sight" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="OptimalDistance" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="RefArmPHYS" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="RefArmEN" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="RefArmHEAT" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ConArmPHYS" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ConArmEN" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ConArmHEAT" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="UpgradeCost" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="UpgradeRequirements" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="SchemeCostMetal" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="SchemeCostEnergy" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Animations" form="unqualified"/>
+                </xsd:sequence>
+                <xsd:attribute name="Workname" form="unqualified" type="xsd:string"/>
+              </xsd:complexType>
+            </xsd:element>
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Upgrade" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="UnitName" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ModelName" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="IconName" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="UnitDescription" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="HpMax" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="HpWreckage" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="HpRegen" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="CostParts" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="CostEnergy" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="CostSM" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="BasicBuildTime" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="DeployRadius" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="SpeedGlobal" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Speed" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ReverseFactor" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="TurnSpeed" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Acceleration" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Mass" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Recovery" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Class" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Priority" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Sight" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="OptimalDistance" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="RefArmPHYS" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="RefArmEN" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="RefArmHEAT" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ConArmPHYS" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ConArmEN" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="ConArmHEAT" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="UpgradeCost" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="UpgradeRequirements" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="UpgradeCategory" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="SchemeCostMetal" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="SchemeCostEnergy" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Animations" form="unqualified"/>
+                </xsd:sequence>
+                <xsd:attribute name="Workname" form="unqualified" type="xsd:string"/>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
   <Map ID="1" Name="Stats_карта" RootElement="Stats" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
+  </Map>
+  <Map ID="2" Name="units_Map" RootElement="units" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1102,9 +1209,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1139,7 +1246,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1174,7 +1281,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1350,23 +1457,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" customWidth="1"/>
+    <col min="20" max="20" width="7.85546875" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" customWidth="1"/>
+    <col min="24" max="24" width="7.7109375" customWidth="1"/>
+    <col min="25" max="25" width="18.140625" customWidth="1"/>
+    <col min="26" max="26" width="14.5703125" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" customWidth="1"/>
+    <col min="29" max="29" width="15" customWidth="1"/>
+    <col min="30" max="30" width="12.85546875" customWidth="1"/>
+    <col min="31" max="31" width="15" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="33" max="33" width="23.85546875" customWidth="1"/>
+    <col min="34" max="34" width="19.7109375" customWidth="1"/>
+    <col min="35" max="35" width="20.42578125" customWidth="1"/>
+    <col min="36" max="36" width="13.42578125" customWidth="1"/>
+    <col min="37" max="37" width="18.5703125" customWidth="1"/>
+    <col min="38" max="38" width="13.42578125" customWidth="1"/>
+    <col min="39" max="39" width="15.5703125" customWidth="1"/>
+    <col min="40" max="40" width="28" customWidth="1"/>
+    <col min="41" max="41" width="18.42578125" customWidth="1"/>
+    <col min="42" max="42" width="10.5703125" customWidth="1"/>
+    <col min="43" max="43" width="15.7109375" customWidth="1"/>
+    <col min="44" max="44" width="12.28515625" customWidth="1"/>
+    <col min="45" max="45" width="13.5703125" customWidth="1"/>
+    <col min="46" max="46" width="15.140625" customWidth="1"/>
+    <col min="47" max="47" width="12" customWidth="1"/>
+    <col min="48" max="48" width="18.85546875" customWidth="1"/>
+    <col min="49" max="49" width="17.5703125" customWidth="1"/>
+    <col min="50" max="50" width="16.85546875" customWidth="1"/>
+    <col min="51" max="51" width="10.85546875" customWidth="1"/>
+    <col min="52" max="52" width="18" customWidth="1"/>
+    <col min="53" max="53" width="14.85546875" customWidth="1"/>
+    <col min="54" max="54" width="16.5703125" customWidth="1"/>
+    <col min="55" max="55" width="9.85546875" customWidth="1"/>
+    <col min="56" max="56" width="13.42578125" customWidth="1"/>
+    <col min="57" max="57" width="9.7109375" customWidth="1"/>
+    <col min="58" max="58" width="11.85546875" customWidth="1"/>
+    <col min="59" max="59" width="9.7109375" customWidth="1"/>
+    <col min="60" max="60" width="20.28515625" customWidth="1"/>
+    <col min="61" max="61" width="16.7109375" customWidth="1"/>
+    <col min="62" max="62" width="14.42578125" customWidth="1"/>
+    <col min="63" max="63" width="16.7109375" customWidth="1"/>
+    <col min="64" max="64" width="17.140625" customWidth="1"/>
+    <col min="65" max="65" width="14.85546875" customWidth="1"/>
+    <col min="66" max="66" width="17.140625" customWidth="1"/>
+    <col min="67" max="67" width="16.85546875" customWidth="1"/>
+    <col min="68" max="68" width="25.85546875" customWidth="1"/>
+    <col min="69" max="69" width="18.85546875" customWidth="1"/>
+    <col min="70" max="70" width="21.7109375" customWidth="1"/>
+    <col min="71" max="71" width="22.42578125" customWidth="1"/>
+    <col min="72" max="72" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>